<commit_message>
Changes after formula import fix
</commit_message>
<xml_diff>
--- a/storage/imports/categories.xlsx
+++ b/storage/imports/categories.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -31,13 +31,43 @@
     <t>Perros</t>
   </si>
   <si>
+    <t>Merchant</t>
+  </si>
+  <si>
     <t>asd</t>
   </si>
   <si>
     <t>Gatos</t>
   </si>
   <si>
-    <t>Finca</t>
+    <t>Otros animales domesticos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alimentos </t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Aseo y belleza animal</t>
+  </si>
+  <si>
+    <t>Servicios veterinarios</t>
+  </si>
+  <si>
+    <t>Juguetes y accesorios</t>
+  </si>
+  <si>
+    <t>Servicios especializados</t>
+  </si>
+  <si>
+    <t>Destacados</t>
+  </si>
+  <si>
+    <t>FAQs</t>
+  </si>
+  <si>
+    <t>Article</t>
   </si>
   <si>
     <t>Documentacion</t>
@@ -59,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -68,6 +98,18 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font/>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <color rgb="FF999999"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF999999"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,14 +126,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -307,6 +361,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="25.0"/>
+    <col customWidth="1" min="6" max="6" width="20.57"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -332,14 +390,14 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>1.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -348,17 +406,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="str">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="str">
         <f t="shared" ref="C3:E3" si="1">C2</f>
-        <v>asd</v>
-      </c>
-      <c r="D3" s="2">
+        <v>Merchant</v>
+      </c>
+      <c r="D3" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="E3" s="3" t="str">
         <f t="shared" si="1"/>
         <v>asd</v>
       </c>
@@ -368,18 +426,18 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="str">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="str">
         <f t="shared" ref="C4:E4" si="3">C3</f>
-        <v>asd</v>
-      </c>
-      <c r="D4" s="2">
+        <v>Merchant</v>
+      </c>
+      <c r="D4" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="str">
+      <c r="E4" s="3" t="str">
         <f t="shared" si="3"/>
         <v>asd</v>
       </c>
@@ -390,17 +448,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="str">
-        <f t="shared" ref="C5:E5" si="4">C4</f>
-        <v>asd</v>
-      </c>
-      <c r="D5" s="2">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:E5" si="4">D4</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="str">
         <f t="shared" si="4"/>
         <v>asd</v>
       </c>
@@ -411,17 +468,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="str">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="str">
         <f t="shared" ref="C6:E6" si="5">C5</f>
-        <v>asd</v>
-      </c>
-      <c r="D6" s="2">
+        <v>Product</v>
+      </c>
+      <c r="D6" s="3">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="str">
+      <c r="E6" s="3" t="str">
         <f t="shared" si="5"/>
         <v>asd</v>
       </c>
@@ -432,17 +489,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="str">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="str">
         <f t="shared" ref="C7:E7" si="6">C6</f>
-        <v>asd</v>
-      </c>
-      <c r="D7" s="2">
+        <v>Product</v>
+      </c>
+      <c r="D7" s="3">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="str">
+      <c r="E7" s="3" t="str">
         <f t="shared" si="6"/>
         <v>asd</v>
       </c>
@@ -453,17 +510,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="str">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="str">
         <f t="shared" ref="C8:E8" si="7">C7</f>
-        <v>asd</v>
-      </c>
-      <c r="D8" s="2">
+        <v>Product</v>
+      </c>
+      <c r="D8" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="str">
+      <c r="E8" s="3" t="str">
         <f t="shared" si="7"/>
         <v>asd</v>
       </c>
@@ -473,20 +530,99 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="str">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="str">
         <f t="shared" ref="C9:E9" si="8">C8</f>
-        <v>asd</v>
-      </c>
-      <c r="D9" s="2">
+        <v>Product</v>
+      </c>
+      <c r="D9" s="3">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="E9" s="2" t="str">
+      <c r="E9" s="3" t="str">
         <f t="shared" si="8"/>
         <v>asd</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f t="shared" ref="C10:E10" si="9">C9</f>
+        <v>Product</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>asd</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ref="D11:E11" si="10">D10</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="str">
+        <f t="shared" si="10"/>
+        <v>asd</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15">
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>